<commit_message>
fixed restaurant logo logos loading issue
</commit_message>
<xml_diff>
--- a/restaurant_data.xlsx
+++ b/restaurant_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dhiraagu-my.sharepoint.com/personal/maail_02624_dhiraagu_com_mv/Documents/personal/roadhaonline/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dhiraagu-my.sharepoint.com/personal/maail_02624_dhiraagu_com_mv/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="82" documentId="8_{F8F3699D-6333-4299-8B41-2205923FDA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12CCFAB1-AC0F-4A90-8C2A-4A7514B46372}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="8_{F8F3699D-6333-4299-8B41-2205923FDA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BA6418C-6925-4C1B-B0DF-172C263A2F3B}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1710" windowWidth="29040" windowHeight="15720" xr2:uid="{D14014FB-EFB2-4719-9A66-74152C34B487}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{D14014FB-EFB2-4719-9A66-74152C34B487}"/>
   </bookViews>
   <sheets>
     <sheet name="restaurant_list" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1744" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1738" uniqueCount="246">
   <si>
     <t>Nuts / Water</t>
   </si>
@@ -754,12 +754,6 @@
     <t>images/mamak/mamak_banner.png</t>
   </si>
   <si>
-    <t>bombay dharbar</t>
-  </si>
-  <si>
-    <t>the island kitchen</t>
-  </si>
-  <si>
     <t>citron</t>
   </si>
   <si>
@@ -772,31 +766,19 @@
     <t>house of flavors</t>
   </si>
   <si>
-    <t>images/house_of_flavors/logo.jpg</t>
-  </si>
-  <si>
-    <t>images/house_of_flavors/banner.jpg</t>
-  </si>
-  <si>
     <t>Acha's Poppadums</t>
   </si>
   <si>
-    <t>images/achaas/logo.png</t>
-  </si>
-  <si>
-    <t>images/achaas/banner.png</t>
-  </si>
-  <si>
-    <t>images/bombay_dharbar/bombay_dharbar_logo.png</t>
-  </si>
-  <si>
-    <t>images/bombay_dharbar/bombay_dharbar_banner.png</t>
-  </si>
-  <si>
-    <t>images/the_island_kitchen/the_island_kitchen_logo.jpg</t>
-  </si>
-  <si>
-    <t>images/the_island_kitchen/the_island_kitchen_banner.jpg</t>
+    <t>images/house_of_flavors/house_of_flavors_logo.png</t>
+  </si>
+  <si>
+    <t>images/house_of_flavors/house_of_flavors_banner.png</t>
+  </si>
+  <si>
+    <t>images/acha's_poppodums/acha's_poppodums_logo.png</t>
+  </si>
+  <si>
+    <t>images/acha's_poppodums/acha's_poppodums_banner.png</t>
   </si>
 </sst>
 </file>
@@ -858,10 +840,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1181,10 +1159,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA06C4E-D4C8-4C24-9F63-95F191572C1F}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,63 +1206,41 @@
         <v>237</v>
       </c>
       <c r="B3" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="C3" t="s">
-        <v>249</v>
+        <v>239</v>
+      </c>
+      <c r="D3" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B4" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="C4" t="s">
-        <v>251</v>
+        <v>243</v>
+      </c>
+      <c r="D4" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B5" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="C5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D5" t="s">
         <v>241</v>
-      </c>
-      <c r="D5" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>242</v>
-      </c>
-      <c r="B6" t="s">
-        <v>243</v>
-      </c>
-      <c r="C6" t="s">
-        <v>244</v>
-      </c>
-      <c r="D6" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>245</v>
-      </c>
-      <c r="B7" t="s">
-        <v>246</v>
-      </c>
-      <c r="C7" t="s">
-        <v>247</v>
-      </c>
-      <c r="D7" t="s">
-        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
there were empty spaces in "resuarant name" in the collumn of excel. also gonna update the index to fix that bug
</commit_message>
<xml_diff>
--- a/restaurant_data.xlsx
+++ b/restaurant_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dhiraagu-my.sharepoint.com/personal/maail_02624_dhiraagu_com_mv/Documents/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="8_{F8F3699D-6333-4299-8B41-2205923FDA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BA6418C-6925-4C1B-B0DF-172C263A2F3B}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{F8F3699D-6333-4299-8B41-2205923FDA96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8CF4E3C-740C-45DC-8E56-CECB930C843E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{D14014FB-EFB2-4719-9A66-74152C34B487}"/>
   </bookViews>
@@ -733,9 +733,6 @@
     <t>Schezwan Chicken</t>
   </si>
   <si>
-    <t xml:space="preserve">restaurant_name  </t>
-  </si>
-  <si>
     <t>logo_path</t>
   </si>
   <si>
@@ -779,6 +776,9 @@
   </si>
   <si>
     <t>images/acha's_poppodums/acha's_poppodums_banner.png</t>
+  </si>
+  <si>
+    <t>restaurant_name</t>
   </si>
 </sst>
 </file>
@@ -840,6 +840,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1162,7 +1166,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,72 +1179,72 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>245</v>
+      </c>
+      <c r="B1" t="s">
         <v>230</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>231</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>232</v>
-      </c>
-      <c r="D1" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B2" t="s">
         <v>234</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>235</v>
       </c>
-      <c r="C2" t="s">
-        <v>236</v>
-      </c>
       <c r="D2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B3" t="s">
         <v>237</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>238</v>
       </c>
-      <c r="C3" t="s">
-        <v>239</v>
-      </c>
       <c r="D3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B4" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" t="s">
         <v>242</v>
       </c>
-      <c r="C4" t="s">
-        <v>243</v>
-      </c>
       <c r="D4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B5" t="s">
+        <v>243</v>
+      </c>
+      <c r="C5" t="s">
         <v>244</v>
       </c>
-      <c r="C5" t="s">
-        <v>245</v>
-      </c>
       <c r="D5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
   </sheetData>

</xml_diff>